<commit_message>
- added qt (release) libraries
- updated gitignore
- updated question sheet
</commit_message>
<xml_diff>
--- a/x64_dbg_gui/Questions - Answers Sheet.xlsx
+++ b/x64_dbg_gui/Questions - Answers Sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Every time an instruction has been executed by  the debugged process  (Every time the debugger switch from run to pause due to a step over/into action, run till action, …) , is it possible to dump the full process memory?</t>
   </si>
@@ -28,14 +28,50 @@
   </si>
   <si>
     <t>Memory map analyis (Who do that, do you have some info)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">answer: unsigned, size: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sizeof(duint)</t>
+    </r>
+  </si>
+  <si>
+    <t>answer: everything unsigned internally</t>
+  </si>
+  <si>
+    <t>answer: we have dbghelp.dll, it can analyze some stuff and it seems logic to do this in the debugger code no?</t>
+  </si>
+  <si>
+    <t>answer: not possible, it will take too much memory, but it is possible to dump the CIP region every time</t>
+  </si>
+  <si>
+    <t>question: switch to a word file??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,7 +103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -80,9 +116,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -120,7 +156,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -192,7 +228,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -366,40 +402,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+  <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="200.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -409,7 +463,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -421,7 +475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>